<commit_message>
Updated data files to be percent change, added correlation matrix + saving it to file
</commit_message>
<xml_diff>
--- a/Data/EconomicData/MonthlyMilk-BLS.xlsx
+++ b/Data/EconomicData/MonthlyMilk-BLS.xlsx
@@ -5,27 +5,43 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\Documents\CodingProjectsStuff\2023SummerResearch-Inflation\Data\EconomicData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\Documents\CodingProjectsStuff\2023SummerResearch-Inflation\COVID-Inflation\Data\EconomicData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA426057-4C72-40D0-AD11-9BF58774205E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DC3614-433E-4206-BE16-A223BD1E4952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BLS Data Series" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Date</t>
   </si>
   <si>
     <t>MilkPrice</t>
+  </si>
+  <si>
+    <t>MilkPrice%Change</t>
   </si>
 </sst>
 </file>
@@ -89,7 +105,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -99,6 +115,9 @@
     </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -414,27 +433,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B281"/>
+  <dimension ref="A1:C281"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>36526</v>
       </c>
@@ -442,2236 +465,3352 @@
         <v>2.7850000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>36557</v>
       </c>
       <c r="B3" s="1">
         <v>2.7770000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <f>(($B3-$B2)/$B2)*100</f>
+        <v>-0.28725314183123901</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>36586</v>
       </c>
       <c r="B4" s="1">
         <v>2.7480000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <f t="shared" ref="C4:C67" si="0">(($B4-$B3)/$B3)*100</f>
+        <v>-1.0442924018725213</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>36617</v>
       </c>
       <c r="B5" s="1">
         <v>2.7730000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0.90975254730712907</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>36647</v>
       </c>
       <c r="B6" s="1">
         <v>2.782</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0.32455824017309398</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>36678</v>
       </c>
       <c r="B7" s="1">
         <v>2.7629999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>-0.68296189791517359</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>36708</v>
       </c>
       <c r="B8" s="1">
         <v>2.7810000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0.65146579804561122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>36739</v>
       </c>
       <c r="B9" s="1">
         <v>2.8069999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.93491549802228702</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>36770</v>
       </c>
       <c r="B10" s="1">
         <v>2.8090000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>7.1250445315291205E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>36800</v>
       </c>
       <c r="B11" s="1">
         <v>2.8050000000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>-0.14239943040227851</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>36831</v>
       </c>
       <c r="B12" s="1">
         <v>2.7530000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>-1.8538324420677377</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>36861</v>
       </c>
       <c r="B13" s="1">
         <v>2.7850000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>1.1623683254631321</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>36892</v>
       </c>
       <c r="B14" s="1">
         <v>2.8519999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>2.405745062836615</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>36923</v>
       </c>
       <c r="B15" s="1">
         <v>2.847</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>-0.17531556802243667</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>36951</v>
       </c>
       <c r="B16" s="1">
         <v>2.76</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>-3.05584826132772</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>36982</v>
       </c>
       <c r="B17" s="1">
         <v>2.8450000000000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>3.0797101449275512</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>37012</v>
       </c>
       <c r="B18" s="1">
         <v>2.8929999999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>1.6871704745166818</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>37043</v>
       </c>
       <c r="B19" s="1">
         <v>2.911</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>0.62219149671621976</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>37073</v>
       </c>
       <c r="B20" s="1">
         <v>2.9329999999999998</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0.75575403641359662</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>37104</v>
       </c>
       <c r="B21" s="1">
         <v>2.89</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>-1.4660756904193559</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>37135</v>
       </c>
       <c r="B22" s="1">
         <v>2.9409999999999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>1.7647058823529311</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>37165</v>
       </c>
       <c r="B23" s="1">
         <v>2.9540000000000002</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>0.44202652159130729</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>37196</v>
       </c>
       <c r="B24" s="1">
         <v>2.89</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>-2.1665538253215995</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>37226</v>
       </c>
       <c r="B25" s="1">
         <v>2.895</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>0.17301038062283366</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>37257</v>
       </c>
       <c r="B26" s="1">
         <v>2.8119999999999998</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>-2.8670120898100238</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>37288</v>
       </c>
       <c r="B27" s="1">
         <v>2.8069999999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>-0.17780938833570037</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>37316</v>
       </c>
       <c r="B28" s="1">
         <v>2.8159999999999998</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>0.32062700391877086</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>37347</v>
       </c>
       <c r="B29" s="1">
         <v>2.7789999999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>-1.3139204545454519</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>37377</v>
       </c>
       <c r="B30" s="1">
         <v>2.782</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>0.10795250089960827</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>37408</v>
       </c>
       <c r="B31" s="1">
         <v>2.7679999999999998</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>-0.50323508267434347</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>37438</v>
       </c>
       <c r="B32" s="1">
         <v>2.7469999999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>-0.75867052023121062</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>37469</v>
       </c>
       <c r="B33" s="1">
         <v>2.72</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>-0.98289042591917331</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>37500</v>
       </c>
       <c r="B34" s="1">
         <v>2.7280000000000002</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>0.29411764705882376</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>37530</v>
       </c>
       <c r="B35" s="1">
         <v>2.7269999999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>-3.6656891495613415E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>37561</v>
       </c>
       <c r="B36" s="1">
         <v>2.7189999999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>-0.29336266960029361</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>37591</v>
       </c>
       <c r="B37" s="1">
         <v>2.6819999999999999</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>-1.3607944097094493</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>37622</v>
       </c>
       <c r="B38" s="1">
         <v>2.6859999999999999</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>0.1491424310216258</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>37653</v>
       </c>
       <c r="B39" s="1">
         <v>2.6890000000000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>0.11169024571854483</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>37681</v>
       </c>
       <c r="B40" s="1">
         <v>2.6560000000000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>-1.2272220156191862</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>37712</v>
       </c>
       <c r="B41" s="1">
         <v>2.6739999999999999</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>0.67771084337348619</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>37742</v>
       </c>
       <c r="B42" s="1">
         <v>2.6850000000000001</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>0.41136873597607032</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>37773</v>
       </c>
       <c r="B43" s="1">
         <v>2.6760000000000002</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>-0.33519553072625319</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>37803</v>
       </c>
       <c r="B44" s="1">
         <v>2.7080000000000002</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>1.1958146487294479</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>37834</v>
       </c>
       <c r="B45" s="1">
         <v>2.6659999999999999</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>-1.5509601181683994</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>37865</v>
       </c>
       <c r="B46" s="1">
         <v>2.9039999999999999</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>8.9272318079519888</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>37895</v>
       </c>
       <c r="B47" s="1">
         <v>2.9049999999999998</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>3.4435261707985186E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>37926</v>
       </c>
       <c r="B48" s="1">
         <v>2.9369999999999998</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>1.1015490533562833</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>37956</v>
       </c>
       <c r="B49" s="1">
         <v>2.9470000000000001</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>0.34048348655091015</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>37987</v>
       </c>
       <c r="B50" s="1">
         <v>2.879</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>-2.3074312860536161</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>38018</v>
       </c>
       <c r="B51" s="1">
         <v>2.8140000000000001</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>-2.2577283779089941</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>38047</v>
       </c>
       <c r="B52" s="1">
         <v>2.786</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>-0.99502487562189135</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>38078</v>
       </c>
       <c r="B53" s="1">
         <v>2.9060000000000001</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>4.3072505384063211</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>38108</v>
       </c>
       <c r="B54" s="1">
         <v>3.3740000000000001</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>16.10461114934618</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>38139</v>
       </c>
       <c r="B55" s="1">
         <v>3.5739999999999998</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>5.9276822762299863</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>38169</v>
       </c>
       <c r="B56" s="1">
         <v>3.4790000000000001</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>-2.6580861779518679</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>38200</v>
       </c>
       <c r="B57" s="1">
         <v>3.2970000000000002</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>-5.2313883299798771</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>38231</v>
       </c>
       <c r="B58" s="1">
         <v>3.149</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>-4.488929329693665</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>38261</v>
       </c>
       <c r="B59" s="1">
         <v>3.161</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>0.38107335662114988</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>38292</v>
       </c>
       <c r="B60" s="1">
         <v>3.2189999999999999</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>1.8348623853210955</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>38322</v>
       </c>
       <c r="B61" s="1">
         <v>3.2330000000000001</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>0.43491767629699396</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>38353</v>
       </c>
       <c r="B62" s="1">
         <v>3.3039999999999998</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>2.1961026909990635</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>38384</v>
       </c>
       <c r="B63" s="1">
         <v>3.1760000000000002</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>-3.8740920096852207</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>38412</v>
       </c>
       <c r="B64" s="1">
         <v>3.226</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>1.5743073047858887</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>38443</v>
       </c>
       <c r="B65" s="1">
         <v>3.2250000000000001</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>-3.0998140111589894E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>38473</v>
       </c>
       <c r="B66" s="1">
         <v>3.2069999999999999</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>-0.55813953488372836</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>38504</v>
       </c>
       <c r="B67" s="1">
         <v>3.1219999999999999</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C67">
+        <f t="shared" si="0"/>
+        <v>-2.6504521359526025</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>38534</v>
       </c>
       <c r="B68" s="1">
         <v>3.09</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C68">
+        <f t="shared" ref="C68:C131" si="1">(($B68-$B67)/$B67)*100</f>
+        <v>-1.0249839846252411</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>38565</v>
       </c>
       <c r="B69" s="1">
         <v>3.1360000000000001</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C69">
+        <f t="shared" si="1"/>
+        <v>1.4886731391585846</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>38596</v>
       </c>
       <c r="B70" s="1">
         <v>3.133</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C70">
+        <f t="shared" si="1"/>
+        <v>-9.5663265306126066E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>38626</v>
       </c>
       <c r="B71" s="1">
         <v>3.1709999999999998</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C71">
+        <f t="shared" si="1"/>
+        <v>1.2128949888285927</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>38657</v>
       </c>
       <c r="B72" s="1">
         <v>3.2109999999999999</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C72">
+        <f t="shared" si="1"/>
+        <v>1.2614317250078853</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>38687</v>
       </c>
       <c r="B73" s="1">
         <v>3.2410000000000001</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C73">
+        <f t="shared" si="1"/>
+        <v>0.93428838368110401</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>38718</v>
       </c>
       <c r="B74" s="1">
         <v>3.1970000000000001</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C74">
+        <f t="shared" si="1"/>
+        <v>-1.3576056772601062</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>38749</v>
       </c>
       <c r="B75" s="1">
         <v>3.2240000000000002</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C75">
+        <f t="shared" si="1"/>
+        <v>0.84454175789803365</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>38777</v>
       </c>
       <c r="B76" s="1">
         <v>3.161</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C76">
+        <f t="shared" si="1"/>
+        <v>-1.9540942928039751</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>38808</v>
       </c>
       <c r="B77" s="1">
         <v>3.1230000000000002</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C77">
+        <f t="shared" si="1"/>
+        <v>-1.2021512179689913</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>38838</v>
       </c>
       <c r="B78" s="1">
         <v>3.0659999999999998</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C78">
+        <f t="shared" si="1"/>
+        <v>-1.825168107588869</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>38869</v>
       </c>
       <c r="B79" s="1">
         <v>3.0009999999999999</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C79">
+        <f t="shared" si="1"/>
+        <v>-2.120026092628831</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>38899</v>
       </c>
       <c r="B80" s="1">
         <v>3.0830000000000002</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C80">
+        <f t="shared" si="1"/>
+        <v>2.732422525824735</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>38930</v>
       </c>
       <c r="B81" s="1">
         <v>3.0190000000000001</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C81">
+        <f t="shared" si="1"/>
+        <v>-2.0759000973078185</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
         <v>38961</v>
       </c>
       <c r="B82" s="1">
         <v>3.0489999999999999</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C82">
+        <f t="shared" si="1"/>
+        <v>0.99370652533950987</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>38991</v>
       </c>
       <c r="B83" s="1">
         <v>3.0640000000000001</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C83">
+        <f t="shared" si="1"/>
+        <v>0.49196457855034847</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
         <v>39022</v>
       </c>
       <c r="B84" s="1">
         <v>2.9849999999999999</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C84">
+        <f t="shared" si="1"/>
+        <v>-2.5783289817232435</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>39052</v>
       </c>
       <c r="B85" s="1">
         <v>3.004</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C85">
+        <f t="shared" si="1"/>
+        <v>0.63651591289782683</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <v>39083</v>
       </c>
       <c r="B86" s="1">
         <v>3.0670000000000002</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C86">
+        <f t="shared" si="1"/>
+        <v>2.0972037283621892</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>39114</v>
       </c>
       <c r="B87" s="1">
         <v>3.0830000000000002</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C87">
+        <f t="shared" si="1"/>
+        <v>0.5216824258232805</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>39142</v>
       </c>
       <c r="B88" s="1">
         <v>3.0720000000000001</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C88">
+        <f t="shared" si="1"/>
+        <v>-0.35679532922478496</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>39173</v>
       </c>
       <c r="B89" s="1">
         <v>3.1349999999999998</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C89">
+        <f t="shared" si="1"/>
+        <v>2.0507812499999911</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
         <v>39203</v>
       </c>
       <c r="B90" s="1">
         <v>3.2589999999999999</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C90">
+        <f t="shared" si="1"/>
+        <v>3.9553429027113278</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>39234</v>
       </c>
       <c r="B91" s="1">
         <v>3.427</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C91">
+        <f t="shared" si="1"/>
+        <v>5.1549555078244911</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
         <v>39264</v>
       </c>
       <c r="B92" s="1">
         <v>3.7360000000000002</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C92">
+        <f t="shared" si="1"/>
+        <v>9.0166326232856768</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>39295</v>
       </c>
       <c r="B93" s="1">
         <v>3.8069999999999999</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C93">
+        <f t="shared" si="1"/>
+        <v>1.9004282655246181</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
         <v>39326</v>
       </c>
       <c r="B94" s="1">
         <v>3.8410000000000002</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C94">
+        <f t="shared" si="1"/>
+        <v>0.89309167323352379</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>39356</v>
       </c>
       <c r="B95" s="1">
         <v>3.8380000000000001</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C95">
+        <f t="shared" si="1"/>
+        <v>-7.8104660244730895E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <v>39387</v>
       </c>
       <c r="B96" s="1">
         <v>3.9039999999999999</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C96">
+        <f t="shared" si="1"/>
+        <v>1.7196456487753995</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>39417</v>
       </c>
       <c r="B97" s="1">
         <v>3.87</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C97">
+        <f t="shared" si="1"/>
+        <v>-0.87090163934425735</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
         <v>39448</v>
       </c>
       <c r="B98" s="1">
         <v>3.871</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C98">
+        <f t="shared" si="1"/>
+        <v>2.5839793281650897E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
         <v>39479</v>
       </c>
       <c r="B99" s="1">
         <v>3.8690000000000002</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C99">
+        <f t="shared" si="1"/>
+        <v>-5.1666236114693349E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
         <v>39508</v>
       </c>
       <c r="B100" s="1">
         <v>3.7810000000000001</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C100">
+        <f t="shared" si="1"/>
+        <v>-2.2744895321788592</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>39539</v>
       </c>
       <c r="B101" s="1">
         <v>3.7989999999999999</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C101">
+        <f t="shared" si="1"/>
+        <v>0.47606453319227165</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
         <v>39569</v>
       </c>
       <c r="B102" s="1">
         <v>3.76</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C102">
+        <f t="shared" si="1"/>
+        <v>-1.0265859436693905</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="3">
         <v>39600</v>
       </c>
       <c r="B103" s="1">
         <v>3.7730000000000001</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C103">
+        <f t="shared" si="1"/>
+        <v>0.34574468085107302</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="3">
         <v>39630</v>
       </c>
       <c r="B104" s="1">
         <v>3.9609999999999999</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C104">
+        <f t="shared" si="1"/>
+        <v>4.9827723297110982</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="3">
         <v>39661</v>
       </c>
       <c r="B105" s="1">
         <v>3.8860000000000001</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C105">
+        <f t="shared" si="1"/>
+        <v>-1.8934612471598014</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="3">
         <v>39692</v>
       </c>
       <c r="B106" s="1">
         <v>3.7730000000000001</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C106">
+        <f t="shared" si="1"/>
+        <v>-2.9078744209984557</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="3">
         <v>39722</v>
       </c>
       <c r="B107" s="1">
         <v>3.6560000000000001</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C107">
+        <f t="shared" si="1"/>
+        <v>-3.1009806520010597</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="3">
         <v>39753</v>
       </c>
       <c r="B108" s="1">
         <v>3.734</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C108">
+        <f t="shared" si="1"/>
+        <v>2.1334792122538251</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="3">
         <v>39783</v>
       </c>
       <c r="B109" s="1">
         <v>3.681</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C109">
+        <f t="shared" si="1"/>
+        <v>-1.4193893947509357</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="3">
         <v>39814</v>
       </c>
       <c r="B110" s="1">
         <v>3.5750000000000002</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C110">
+        <f t="shared" si="1"/>
+        <v>-2.8796522684053212</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
         <v>39845</v>
       </c>
       <c r="B111" s="1">
         <v>3.319</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C111">
+        <f t="shared" si="1"/>
+        <v>-7.1608391608391662</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="3">
         <v>39873</v>
       </c>
       <c r="B112" s="1">
         <v>3.1160000000000001</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C112">
+        <f t="shared" si="1"/>
+        <v>-6.1163000903886671</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
         <v>39904</v>
       </c>
       <c r="B113" s="1">
         <v>3.0840000000000001</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C113">
+        <f t="shared" si="1"/>
+        <v>-1.0269576379974334</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
         <v>39934</v>
       </c>
       <c r="B114" s="1">
         <v>3.0680000000000001</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C114">
+        <f t="shared" si="1"/>
+        <v>-0.51880674448767872</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
         <v>39965</v>
       </c>
       <c r="B115" s="1">
         <v>3.0089999999999999</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C115">
+        <f t="shared" si="1"/>
+        <v>-1.9230769230769285</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="3">
         <v>39995</v>
       </c>
       <c r="B116" s="1">
         <v>2.992</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C116">
+        <f t="shared" si="1"/>
+        <v>-0.56497175141242617</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="3">
         <v>40026</v>
       </c>
       <c r="B117" s="1">
         <v>2.9790000000000001</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C117">
+        <f t="shared" si="1"/>
+        <v>-0.43449197860962235</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="3">
         <v>40057</v>
       </c>
       <c r="B118" s="1">
         <v>2.9809999999999999</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C118">
+        <f t="shared" si="1"/>
+        <v>6.7136623027854309E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>40087</v>
       </c>
       <c r="B119" s="1">
         <v>3.0459999999999998</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C119">
+        <f t="shared" si="1"/>
+        <v>2.1804763502180458</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
         <v>40118</v>
       </c>
       <c r="B120" s="1">
         <v>3.0339999999999998</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C120">
+        <f t="shared" si="1"/>
+        <v>-0.39395929087327686</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
         <v>40148</v>
       </c>
       <c r="B121" s="1">
         <v>3.105</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C121">
+        <f t="shared" si="1"/>
+        <v>2.3401450230718583</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
         <v>40179</v>
       </c>
       <c r="B122" s="1">
         <v>3.2360000000000002</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C122">
+        <f t="shared" si="1"/>
+        <v>4.2190016103059653</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
         <v>40210</v>
       </c>
       <c r="B123" s="1">
         <v>3.2029999999999998</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C123">
+        <f t="shared" si="1"/>
+        <v>-1.0197775030902461</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
         <v>40238</v>
       </c>
       <c r="B124" s="1">
         <v>3.1880000000000002</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C124">
+        <f t="shared" si="1"/>
+        <v>-0.46831095847641835</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>40269</v>
       </c>
       <c r="B125" s="1">
         <v>3.14</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C125">
+        <f t="shared" si="1"/>
+        <v>-1.5056461731493112</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="3">
         <v>40299</v>
       </c>
       <c r="B126" s="1">
         <v>3.1779999999999999</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C126">
+        <f t="shared" si="1"/>
+        <v>1.2101910828025417</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="3">
         <v>40330</v>
       </c>
       <c r="B127" s="1">
         <v>3.2970000000000002</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C127">
+        <f t="shared" si="1"/>
+        <v>3.7444933920704915</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="3">
         <v>40360</v>
       </c>
       <c r="B128" s="1">
         <v>3.3130000000000002</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C128">
+        <f t="shared" si="1"/>
+        <v>0.48528965726418</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="3">
         <v>40391</v>
       </c>
       <c r="B129" s="1">
         <v>3.3029999999999999</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C129">
+        <f t="shared" si="1"/>
+        <v>-0.30184123151223152</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="3">
         <v>40422</v>
       </c>
       <c r="B130" s="1">
         <v>3.278</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C130">
+        <f t="shared" si="1"/>
+        <v>-0.75688767786860167</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
         <v>40452</v>
       </c>
       <c r="B131" s="1">
         <v>3.3210000000000002</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C131">
+        <f t="shared" si="1"/>
+        <v>1.311775472849303</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="3">
         <v>40483</v>
       </c>
       <c r="B132" s="1">
         <v>3.327</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C132">
+        <f t="shared" ref="C132:C195" si="2">(($B132-$B131)/$B131)*100</f>
+        <v>0.18066847335139363</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="3">
         <v>40513</v>
       </c>
       <c r="B133" s="1">
         <v>3.3180000000000001</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C133">
+        <f t="shared" si="2"/>
+        <v>-0.27051397655545228</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="3">
         <v>40544</v>
       </c>
       <c r="B134" s="1">
         <v>3.3010000000000002</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C134">
+        <f t="shared" si="2"/>
+        <v>-0.51235684147076266</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="3">
         <v>40575</v>
       </c>
       <c r="B135" s="1">
         <v>3.3570000000000002</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C135">
+        <f t="shared" si="2"/>
+        <v>1.6964556195092411</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="3">
         <v>40603</v>
       </c>
       <c r="B136" s="1">
         <v>3.5030000000000001</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C136">
+        <f t="shared" si="2"/>
+        <v>4.3491212392016649</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="3">
         <v>40634</v>
       </c>
       <c r="B137" s="1">
         <v>3.597</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C137">
+        <f t="shared" si="2"/>
+        <v>2.6834142163859509</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="3">
         <v>40664</v>
       </c>
       <c r="B138" s="1">
         <v>3.653</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C138">
+        <f t="shared" si="2"/>
+        <v>1.5568529329997234</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="3">
         <v>40695</v>
       </c>
       <c r="B139" s="1">
         <v>3.6219999999999999</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C139">
+        <f t="shared" si="2"/>
+        <v>-0.84861757459622611</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="3">
         <v>40725</v>
       </c>
       <c r="B140" s="1">
         <v>3.6539999999999999</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C140">
+        <f t="shared" si="2"/>
+        <v>0.88348978464936578</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="3">
         <v>40756</v>
       </c>
       <c r="B141" s="1">
         <v>3.7130000000000001</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C141">
+        <f t="shared" si="2"/>
+        <v>1.614668856048171</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="3">
         <v>40787</v>
       </c>
       <c r="B142" s="1">
         <v>3.7149999999999999</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C142">
+        <f t="shared" si="2"/>
+        <v>5.3864799353616474E-2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" s="3">
         <v>40817</v>
       </c>
       <c r="B143" s="1">
         <v>3.6219999999999999</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C143">
+        <f t="shared" si="2"/>
+        <v>-2.5033647375504704</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="3">
         <v>40848</v>
       </c>
       <c r="B144" s="1">
         <v>3.5569999999999999</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C144">
+        <f t="shared" si="2"/>
+        <v>-1.7945886250690213</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="3">
         <v>40878</v>
       </c>
       <c r="B145" s="1">
         <v>3.5649999999999999</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C145">
+        <f t="shared" si="2"/>
+        <v>0.2249086308687098</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="3">
         <v>40909</v>
       </c>
       <c r="B146" s="1">
         <v>3.5830000000000002</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C146">
+        <f t="shared" si="2"/>
+        <v>0.50490883590463498</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="3">
         <v>40940</v>
       </c>
       <c r="B147" s="1">
         <v>3.52</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C147">
+        <f t="shared" si="2"/>
+        <v>-1.7583030979626058</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="3">
         <v>40969</v>
       </c>
       <c r="B148" s="1">
         <v>3.4990000000000001</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C148">
+        <f t="shared" si="2"/>
+        <v>-0.5965909090909064</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="3">
         <v>41000</v>
       </c>
       <c r="B149" s="1">
         <v>3.4740000000000002</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C149">
+        <f t="shared" si="2"/>
+        <v>-0.71448985424406719</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="3">
         <v>41030</v>
       </c>
       <c r="B150" s="1">
         <v>3.427</v>
       </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C150">
+        <f t="shared" si="2"/>
+        <v>-1.3529073114565386</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="3">
         <v>41061</v>
       </c>
       <c r="B151" s="1">
         <v>3.3959999999999999</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C151">
+        <f t="shared" si="2"/>
+        <v>-0.9045812664137769</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="3">
         <v>41091</v>
       </c>
       <c r="B152" s="1">
         <v>3.4279999999999999</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C152">
+        <f t="shared" si="2"/>
+        <v>0.94228504122497136</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" s="3">
         <v>41122</v>
       </c>
       <c r="B153" s="1">
         <v>3.4740000000000002</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C153">
+        <f t="shared" si="2"/>
+        <v>1.3418903150525165</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="3">
         <v>41153</v>
       </c>
       <c r="B154" s="1">
         <v>3.4689999999999999</v>
       </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C154">
+        <f t="shared" si="2"/>
+        <v>-0.14392630972942824</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="3">
         <v>41183</v>
       </c>
       <c r="B155" s="1">
         <v>3.524</v>
       </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C155">
+        <f t="shared" si="2"/>
+        <v>1.5854713173825357</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="3">
         <v>41214</v>
       </c>
       <c r="B156" s="1">
         <v>3.536</v>
       </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C156">
+        <f t="shared" si="2"/>
+        <v>0.34052213393870628</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="3">
         <v>41244</v>
       </c>
       <c r="B157" s="1">
         <v>3.58</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C157">
+        <f t="shared" si="2"/>
+        <v>1.2443438914027161</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" s="3">
         <v>41275</v>
       </c>
       <c r="B158" s="1">
         <v>3.5259999999999998</v>
       </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C158">
+        <f t="shared" si="2"/>
+        <v>-1.5083798882681638</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="3">
         <v>41306</v>
       </c>
       <c r="B159" s="1">
         <v>3.48</v>
       </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C159">
+        <f t="shared" si="2"/>
+        <v>-1.3045944412932451</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" s="3">
         <v>41334</v>
       </c>
       <c r="B160" s="1">
         <v>3.431</v>
       </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C160">
+        <f t="shared" si="2"/>
+        <v>-1.4080459770114924</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" s="3">
         <v>41365</v>
       </c>
       <c r="B161" s="1">
         <v>3.4279999999999999</v>
       </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C161">
+        <f t="shared" si="2"/>
+        <v>-8.7438064704171189E-2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" s="3">
         <v>41395</v>
       </c>
       <c r="B162" s="1">
         <v>3.4409999999999998</v>
       </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C162">
+        <f t="shared" si="2"/>
+        <v>0.37922987164527133</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" s="3">
         <v>41426</v>
       </c>
       <c r="B163" s="1">
         <v>3.4580000000000002</v>
       </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C163">
+        <f t="shared" si="2"/>
+        <v>0.49404242952631061</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" s="3">
         <v>41456</v>
       </c>
       <c r="B164" s="1">
         <v>3.4489999999999998</v>
       </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C164">
+        <f t="shared" si="2"/>
+        <v>-0.26026604973974382</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" s="3">
         <v>41487</v>
       </c>
       <c r="B165" s="1">
         <v>3.448</v>
       </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C165">
+        <f t="shared" si="2"/>
+        <v>-2.8993911278628295E-2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="3">
         <v>41518</v>
       </c>
       <c r="B166" s="1">
         <v>3.4279999999999999</v>
       </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C166">
+        <f t="shared" si="2"/>
+        <v>-0.58004640371229743</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" s="3">
         <v>41548</v>
       </c>
       <c r="B167" s="1">
         <v>3.4620000000000002</v>
       </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C167">
+        <f t="shared" si="2"/>
+        <v>0.9918319719953399</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" s="3">
         <v>41579</v>
       </c>
       <c r="B168" s="1">
         <v>3.4910000000000001</v>
       </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C168">
+        <f t="shared" si="2"/>
+        <v>0.83766608896591321</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" s="3">
         <v>41609</v>
       </c>
       <c r="B169" s="1">
         <v>3.5009999999999999</v>
       </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C169">
+        <f t="shared" si="2"/>
+        <v>0.28645087367515859</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" s="3">
         <v>41640</v>
       </c>
       <c r="B170" s="1">
         <v>3.552</v>
       </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C170">
+        <f t="shared" si="2"/>
+        <v>1.4567266495287106</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" s="3">
         <v>41671</v>
       </c>
       <c r="B171" s="1">
         <v>3.5609999999999999</v>
       </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C171">
+        <f t="shared" si="2"/>
+        <v>0.25337837837837551</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" s="3">
         <v>41699</v>
       </c>
       <c r="B172" s="1">
         <v>3.669</v>
       </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C172">
+        <f t="shared" si="2"/>
+        <v>3.032855939342884</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" s="3">
         <v>41730</v>
       </c>
       <c r="B173" s="1">
         <v>3.6869999999999998</v>
       </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C173">
+        <f t="shared" si="2"/>
+        <v>0.49059689288633945</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" s="3">
         <v>41760</v>
       </c>
       <c r="B174" s="1">
         <v>3.7349999999999999</v>
       </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C174">
+        <f t="shared" si="2"/>
+        <v>1.3018714401952818</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" s="3">
         <v>41791</v>
       </c>
       <c r="B175" s="1">
         <v>3.6259999999999999</v>
       </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C175">
+        <f t="shared" si="2"/>
+        <v>-2.9183400267737616</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" s="3">
         <v>41821</v>
       </c>
       <c r="B176" s="1">
         <v>3.645</v>
       </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C176">
+        <f t="shared" si="2"/>
+        <v>0.52399338113624183</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" s="3">
         <v>41852</v>
       </c>
       <c r="B177" s="1">
         <v>3.673</v>
       </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C177">
+        <f t="shared" si="2"/>
+        <v>0.76817558299039856</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" s="3">
         <v>41883</v>
       </c>
       <c r="B178" s="1">
         <v>3.7320000000000002</v>
       </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C178">
+        <f t="shared" si="2"/>
+        <v>1.6063163626463424</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" s="3">
         <v>41913</v>
       </c>
       <c r="B179" s="1">
         <v>3.766</v>
       </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C179">
+        <f t="shared" si="2"/>
+        <v>0.91103965702035927</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" s="3">
         <v>41944</v>
       </c>
       <c r="B180" s="1">
         <v>3.8580000000000001</v>
       </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C180">
+        <f t="shared" si="2"/>
+        <v>2.4429102496017019</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="3">
         <v>41974</v>
       </c>
       <c r="B181" s="1">
         <v>3.82</v>
       </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C181">
+        <f t="shared" si="2"/>
+        <v>-0.98496630378435079</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" s="3">
         <v>42005</v>
       </c>
       <c r="B182" s="1">
         <v>3.758</v>
       </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C182">
+        <f t="shared" si="2"/>
+        <v>-1.6230366492146553</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" s="3">
         <v>42036</v>
       </c>
       <c r="B183" s="1">
         <v>3.496</v>
       </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C183">
+        <f t="shared" si="2"/>
+        <v>-6.9717935071846728</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" s="3">
         <v>42064</v>
       </c>
       <c r="B184" s="1">
         <v>3.4630000000000001</v>
       </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C184">
+        <f t="shared" si="2"/>
+        <v>-0.94393592677345306</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" s="3">
         <v>42095</v>
       </c>
       <c r="B185" s="1">
         <v>3.3969999999999998</v>
       </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C185">
+        <f t="shared" si="2"/>
+        <v>-1.9058619693907097</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" s="3">
         <v>42125</v>
       </c>
       <c r="B186" s="1">
         <v>3.387</v>
       </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C186">
+        <f t="shared" si="2"/>
+        <v>-0.29437739181630224</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" s="3">
         <v>42156</v>
       </c>
       <c r="B187" s="1">
         <v>3.3660000000000001</v>
       </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C187">
+        <f t="shared" si="2"/>
+        <v>-0.62001771479184853</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" s="3">
         <v>42186</v>
       </c>
       <c r="B188" s="1">
         <v>3.43</v>
       </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C188">
+        <f t="shared" si="2"/>
+        <v>1.9013666072489617</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" s="3">
         <v>42217</v>
       </c>
       <c r="B189" s="1">
         <v>3.3889999999999998</v>
       </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C189">
+        <f t="shared" si="2"/>
+        <v>-1.1953352769679408</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" s="3">
         <v>42248</v>
       </c>
       <c r="B190" s="1">
         <v>3.3919999999999999</v>
       </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C190">
+        <f t="shared" si="2"/>
+        <v>8.8521687813517672E-2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" s="3">
         <v>42278</v>
       </c>
       <c r="B191" s="1">
         <v>3.3380000000000001</v>
       </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C191">
+        <f t="shared" si="2"/>
+        <v>-1.5919811320754664</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" s="3">
         <v>42309</v>
       </c>
       <c r="B192" s="1">
         <v>3.2989999999999999</v>
       </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C192">
+        <f t="shared" si="2"/>
+        <v>-1.1683642899940128</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" s="3">
         <v>42339</v>
       </c>
       <c r="B193" s="1">
         <v>3.31</v>
       </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C193">
+        <f t="shared" si="2"/>
+        <v>0.3334343740527469</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" s="3">
         <v>42370</v>
       </c>
       <c r="B194" s="1">
         <v>3.3130000000000002</v>
       </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C194">
+        <f t="shared" si="2"/>
+        <v>9.0634441087616729E-2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" s="3">
         <v>42401</v>
       </c>
       <c r="B195" s="1">
         <v>3.23</v>
       </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C195">
+        <f t="shared" si="2"/>
+        <v>-2.5052822215514694</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" s="3">
         <v>42430</v>
       </c>
       <c r="B196" s="1">
         <v>3.1869999999999998</v>
       </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C196">
+        <f t="shared" ref="C196:C259" si="3">(($B196-$B195)/$B195)*100</f>
+        <v>-1.3312693498452057</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" s="3">
         <v>42461</v>
       </c>
       <c r="B197" s="1">
         <v>3.1549999999999998</v>
       </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C197">
+        <f t="shared" si="3"/>
+        <v>-1.0040790712268601</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" s="3">
         <v>42491</v>
       </c>
       <c r="B198" s="1">
         <v>3.157</v>
       </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C198">
+        <f t="shared" si="3"/>
+        <v>6.3391442155316127E-2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" s="3">
         <v>42522</v>
       </c>
       <c r="B199" s="1">
         <v>3.1150000000000002</v>
       </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C199">
+        <f t="shared" si="3"/>
+        <v>-1.3303769401330319</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" s="3">
         <v>42552</v>
       </c>
       <c r="B200" s="1">
         <v>3.0619999999999998</v>
       </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C200">
+        <f t="shared" si="3"/>
+        <v>-1.7014446227929494</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" s="3">
         <v>42583</v>
       </c>
       <c r="B201" s="1">
         <v>3.141</v>
       </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C201">
+        <f t="shared" si="3"/>
+        <v>2.5800130633572889</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" s="3">
         <v>42614</v>
       </c>
       <c r="B202" s="1">
         <v>3.2290000000000001</v>
       </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C202">
+        <f t="shared" si="3"/>
+        <v>2.8016555237185634</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" s="3">
         <v>42644</v>
       </c>
       <c r="B203" s="1">
         <v>3.2919999999999998</v>
       </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C203">
+        <f t="shared" si="3"/>
+        <v>1.9510684422421716</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" s="3">
         <v>42675</v>
       </c>
       <c r="B204" s="1">
         <v>3.28</v>
       </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C204">
+        <f t="shared" si="3"/>
+        <v>-0.36452004860267351</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" s="3">
         <v>42705</v>
       </c>
       <c r="B205" s="1">
         <v>3.29</v>
       </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C205">
+        <f t="shared" si="3"/>
+        <v>0.3048780487804949</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" s="3">
         <v>42736</v>
       </c>
       <c r="B206" s="1">
         <v>3.3180000000000001</v>
       </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C206">
+        <f t="shared" si="3"/>
+        <v>0.85106382978723472</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" s="3">
         <v>42767</v>
       </c>
       <c r="B207" s="1">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C207">
+        <f t="shared" si="3"/>
+        <v>-0.54249547920434715</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" s="3">
         <v>42795</v>
       </c>
       <c r="B208" s="1">
         <v>3.3149999999999999</v>
       </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C208">
+        <f t="shared" si="3"/>
+        <v>0.45454545454545836</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" s="3">
         <v>42826</v>
       </c>
       <c r="B209" s="1">
         <v>3.2589999999999999</v>
       </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C209">
+        <f t="shared" si="3"/>
+        <v>-1.6892911010558085</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" s="3">
         <v>42856</v>
       </c>
       <c r="B210" s="1">
         <v>3.242</v>
       </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C210">
+        <f t="shared" si="3"/>
+        <v>-0.52163240257747479</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" s="3">
         <v>42887</v>
       </c>
       <c r="B211" s="1">
         <v>3.2130000000000001</v>
       </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C211">
+        <f t="shared" si="3"/>
+        <v>-0.89450956199876364</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" s="3">
         <v>42917</v>
       </c>
       <c r="B212" s="1">
         <v>3.2189999999999999</v>
       </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C212">
+        <f t="shared" si="3"/>
+        <v>0.18674136321194468</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" s="3">
         <v>42948</v>
       </c>
       <c r="B213" s="1">
         <v>3.1680000000000001</v>
       </c>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C213">
+        <f t="shared" si="3"/>
+        <v>-1.5843429636532995</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" s="3">
         <v>42979</v>
       </c>
       <c r="B214" s="1">
         <v>3.2090000000000001</v>
       </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C214">
+        <f t="shared" si="3"/>
+        <v>1.2941919191919167</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" s="3">
         <v>43009</v>
       </c>
       <c r="B215" s="1">
         <v>3.1579999999999999</v>
       </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C215">
+        <f t="shared" si="3"/>
+        <v>-1.589280149579313</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" s="3">
         <v>43040</v>
       </c>
       <c r="B216" s="1">
         <v>3.15</v>
       </c>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C216">
+        <f t="shared" si="3"/>
+        <v>-0.25332488917036122</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" s="3">
         <v>43070</v>
       </c>
       <c r="B217" s="1">
         <v>3.1549999999999998</v>
       </c>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C217">
+        <f t="shared" si="3"/>
+        <v>0.15873015873015534</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" s="3">
         <v>43101</v>
       </c>
       <c r="B218" s="1">
         <v>2.9609999999999999</v>
       </c>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C218">
+        <f t="shared" si="3"/>
+        <v>-6.1489698890649747</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" s="3">
         <v>43132</v>
       </c>
       <c r="B219" s="1">
         <v>2.923</v>
       </c>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C219">
+        <f t="shared" si="3"/>
+        <v>-1.2833502195204258</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" s="3">
         <v>43160</v>
       </c>
       <c r="B220" s="1">
         <v>2.903</v>
       </c>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C220">
+        <f t="shared" si="3"/>
+        <v>-0.68422853232979874</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" s="3">
         <v>43191</v>
       </c>
       <c r="B221" s="1">
         <v>2.9239999999999999</v>
       </c>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C221">
+        <f t="shared" si="3"/>
+        <v>0.72338959696864991</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" s="3">
         <v>43221</v>
       </c>
       <c r="B222" s="1">
         <v>2.919</v>
       </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C222">
+        <f t="shared" si="3"/>
+        <v>-0.17099863201094026</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" s="3">
         <v>43252</v>
       </c>
       <c r="B223" s="1">
         <v>2.8769999999999998</v>
       </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C223">
+        <f t="shared" si="3"/>
+        <v>-1.4388489208633182</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" s="3">
         <v>43282</v>
       </c>
       <c r="B224" s="1">
         <v>2.839</v>
       </c>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C224">
+        <f t="shared" si="3"/>
+        <v>-1.3208202989224822</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" s="3">
         <v>43313</v>
       </c>
       <c r="B225" s="1">
         <v>2.871</v>
       </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C225">
+        <f t="shared" si="3"/>
+        <v>1.1271574498062709</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" s="3">
         <v>43344</v>
       </c>
       <c r="B226" s="1">
         <v>2.89</v>
       </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C226">
+        <f t="shared" si="3"/>
+        <v>0.66179031696273516</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" s="3">
         <v>43374</v>
       </c>
       <c r="B227" s="1">
         <v>2.9129999999999998</v>
       </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C227">
+        <f t="shared" si="3"/>
+        <v>0.795847750865041</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" s="3">
         <v>43405</v>
       </c>
       <c r="B228" s="1">
         <v>2.8769999999999998</v>
       </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C228">
+        <f t="shared" si="3"/>
+        <v>-1.235839340885686</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" s="3">
         <v>43435</v>
       </c>
       <c r="B229" s="1">
         <v>2.8530000000000002</v>
       </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C229">
+        <f t="shared" si="3"/>
+        <v>-0.83420229405629409</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" s="3">
         <v>43466</v>
       </c>
       <c r="B230" s="1">
         <v>2.9129999999999998</v>
       </c>
-    </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C230">
+        <f t="shared" si="3"/>
+        <v>2.1030494216613951</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" s="3">
         <v>43497</v>
       </c>
       <c r="B231" s="1">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C231">
+        <f t="shared" si="3"/>
+        <v>-0.44627531754204947</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" s="3">
         <v>43525</v>
       </c>
       <c r="B232" s="1">
         <v>2.944</v>
       </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C232">
+        <f t="shared" si="3"/>
+        <v>1.5172413793103463</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" s="3">
         <v>43556</v>
       </c>
       <c r="B233" s="1">
         <v>2.98</v>
       </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C233">
+        <f t="shared" si="3"/>
+        <v>1.2228260869565228</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" s="3">
         <v>43586</v>
       </c>
       <c r="B234" s="1">
         <v>2.9630000000000001</v>
       </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C234">
+        <f t="shared" si="3"/>
+        <v>-0.57046979865771485</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" s="3">
         <v>43617</v>
       </c>
       <c r="B235" s="1">
         <v>3.0539999999999998</v>
       </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C235">
+        <f t="shared" si="3"/>
+        <v>3.0712116098548679</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" s="3">
         <v>43647</v>
       </c>
       <c r="B236" s="1">
         <v>3.0310000000000001</v>
       </c>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C236">
+        <f t="shared" si="3"/>
+        <v>-0.75311067452520264</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" s="3">
         <v>43678</v>
       </c>
       <c r="B237" s="1">
         <v>3.0449999999999999</v>
       </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C237">
+        <f t="shared" si="3"/>
+        <v>0.46189376443417318</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" s="3">
         <v>43709</v>
       </c>
       <c r="B238" s="1">
         <v>3.1019999999999999</v>
       </c>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C238">
+        <f t="shared" si="3"/>
+        <v>1.8719211822660078</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" s="3">
         <v>43739</v>
       </c>
       <c r="B239" s="1">
         <v>3.1190000000000002</v>
       </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C239">
+        <f t="shared" si="3"/>
+        <v>0.54803352675694228</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" s="3">
         <v>43770</v>
       </c>
       <c r="B240" s="1">
         <v>3.1890000000000001</v>
       </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C240">
+        <f t="shared" si="3"/>
+        <v>2.244309073420963</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" s="3">
         <v>43800</v>
       </c>
       <c r="B241" s="1">
         <v>3.1880000000000002</v>
       </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C241">
+        <f t="shared" si="3"/>
+        <v>-3.1357792411410783E-2</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" s="3">
         <v>43831</v>
       </c>
       <c r="B242" s="1">
         <v>3.2530000000000001</v>
       </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C242">
+        <f t="shared" si="3"/>
+        <v>2.0388958594730222</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" s="3">
         <v>43862</v>
       </c>
       <c r="B243" s="1">
         <v>3.1960000000000002</v>
       </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C243">
+        <f t="shared" si="3"/>
+        <v>-1.7522287119581905</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244" s="3">
         <v>43891</v>
       </c>
       <c r="B244" s="1">
         <v>3.2480000000000002</v>
       </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C244">
+        <f t="shared" si="3"/>
+        <v>1.6270337922403018</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245" s="3">
         <v>43922</v>
       </c>
       <c r="B245" s="1">
         <v>3.2669999999999999</v>
       </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C245">
+        <f t="shared" si="3"/>
+        <v>0.58497536945811834</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" s="3">
         <v>43952</v>
       </c>
       <c r="B246" s="1">
         <v>3.21</v>
       </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C246">
+        <f t="shared" si="3"/>
+        <v>-1.7447199265381064</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247" s="3">
         <v>43983</v>
       </c>
       <c r="B247" s="1">
         <v>3.198</v>
       </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C247">
+        <f t="shared" si="3"/>
+        <v>-0.3738317757009349</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248" s="3">
         <v>44013</v>
       </c>
       <c r="B248" s="1">
         <v>3.2549999999999999</v>
       </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C248">
+        <f t="shared" si="3"/>
+        <v>1.782363977485927</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249" s="3">
         <v>44044</v>
       </c>
       <c r="B249" s="1">
         <v>3.4060000000000001</v>
       </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C249">
+        <f t="shared" si="3"/>
+        <v>4.6390168970814205</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250" s="3">
         <v>44075</v>
       </c>
       <c r="B250" s="1">
         <v>3.448</v>
       </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C250">
+        <f t="shared" si="3"/>
+        <v>1.2331180270111513</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251" s="3">
         <v>44105</v>
       </c>
       <c r="B251" s="1">
         <v>3.38</v>
       </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C251">
+        <f t="shared" si="3"/>
+        <v>-1.9721577726218114</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252" s="3">
         <v>44136</v>
       </c>
       <c r="B252" s="1">
         <v>3.4249999999999998</v>
       </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C252">
+        <f t="shared" si="3"/>
+        <v>1.33136094674556</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253" s="3">
         <v>44166</v>
       </c>
       <c r="B253" s="1">
         <v>3.5350000000000001</v>
       </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C253">
+        <f t="shared" si="3"/>
+        <v>3.2116788321167982</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" s="3">
         <v>44197</v>
       </c>
       <c r="B254" s="1">
         <v>3.468</v>
       </c>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C254">
+        <f t="shared" si="3"/>
+        <v>-1.8953323903818999</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255" s="3">
         <v>44228</v>
       </c>
       <c r="B255" s="1">
         <v>3.3679999999999999</v>
       </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C255">
+        <f t="shared" si="3"/>
+        <v>-2.8835063437139588</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A256" s="3">
         <v>44256</v>
       </c>
       <c r="B256" s="1">
         <v>3.3479999999999999</v>
       </c>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C256">
+        <f t="shared" si="3"/>
+        <v>-0.59382422802850421</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A257" s="3">
         <v>44287</v>
       </c>
       <c r="B257" s="1">
         <v>3.4470000000000001</v>
       </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C257">
+        <f t="shared" si="3"/>
+        <v>2.9569892473118342</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A258" s="3">
         <v>44317</v>
       </c>
       <c r="B258" s="1">
         <v>3.4969999999999999</v>
       </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C258">
+        <f t="shared" si="3"/>
+        <v>1.4505366985784689</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A259" s="3">
         <v>44348</v>
       </c>
       <c r="B259" s="1">
         <v>3.5569999999999999</v>
       </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C259">
+        <f t="shared" si="3"/>
+        <v>1.7157563625965127</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A260" s="3">
         <v>44378</v>
       </c>
       <c r="B260" s="1">
         <v>3.6269999999999998</v>
       </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C260">
+        <f t="shared" ref="C260:C281" si="4">(($B260-$B259)/$B259)*100</f>
+        <v>1.9679505201012044</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A261" s="3">
         <v>44409</v>
       </c>
       <c r="B261" s="1">
         <v>3.56</v>
       </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C261">
+        <f t="shared" si="4"/>
+        <v>-1.8472566859663559</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A262" s="3">
         <v>44440</v>
       </c>
       <c r="B262" s="1">
         <v>3.585</v>
       </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C262">
+        <f t="shared" si="4"/>
+        <v>0.70224719101123345</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A263" s="3">
         <v>44470</v>
       </c>
       <c r="B263" s="1">
         <v>3.6629999999999998</v>
       </c>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C263">
+        <f t="shared" si="4"/>
+        <v>2.1757322175732172</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A264" s="3">
         <v>44501</v>
       </c>
       <c r="B264" s="1">
         <v>3.6709999999999998</v>
       </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C264">
+        <f t="shared" si="4"/>
+        <v>0.21840021840021859</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A265" s="3">
         <v>44531</v>
       </c>
       <c r="B265" s="1">
         <v>3.7429999999999999</v>
       </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C265">
+        <f t="shared" si="4"/>
+        <v>1.9613184418414618</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A266" s="3">
         <v>44562</v>
       </c>
       <c r="B266" s="1">
         <v>3.7869999999999999</v>
       </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C266">
+        <f t="shared" si="4"/>
+        <v>1.1755276516163518</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A267" s="3">
         <v>44593</v>
       </c>
       <c r="B267" s="1">
         <v>3.875</v>
       </c>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C267">
+        <f t="shared" si="4"/>
+        <v>2.3237391074729357</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A268" s="3">
         <v>44621</v>
       </c>
       <c r="B268" s="1">
         <v>3.9169999999999998</v>
       </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C268">
+        <f t="shared" si="4"/>
+        <v>1.0838709677419307</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A269" s="3">
         <v>44652</v>
       </c>
       <c r="B269" s="1">
         <v>4.0119999999999996</v>
       </c>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C269">
+        <f t="shared" si="4"/>
+        <v>2.4253255042124011</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A270" s="3">
         <v>44682</v>
       </c>
       <c r="B270" s="1">
         <v>4.2039999999999997</v>
       </c>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C270">
+        <f t="shared" si="4"/>
+        <v>4.7856430707876418</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A271" s="3">
         <v>44713</v>
       </c>
       <c r="B271" s="1">
         <v>4.1529999999999996</v>
       </c>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C271">
+        <f t="shared" si="4"/>
+        <v>-1.2131303520456747</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A272" s="3">
         <v>44743</v>
       </c>
       <c r="B272" s="1">
         <v>4.1559999999999997</v>
       </c>
-    </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C272">
+        <f t="shared" si="4"/>
+        <v>7.223693715386742E-2</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A273" s="3">
         <v>44774</v>
       </c>
       <c r="B273" s="1">
         <v>4.194</v>
       </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C273">
+        <f t="shared" si="4"/>
+        <v>0.91434071222329782</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A274" s="3">
         <v>44805</v>
       </c>
       <c r="B274" s="1">
         <v>4.181</v>
       </c>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C274">
+        <f t="shared" si="4"/>
+        <v>-0.30996661897949218</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A275" s="3">
         <v>44835</v>
       </c>
       <c r="B275" s="1">
         <v>4.1840000000000002</v>
       </c>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C275">
+        <f t="shared" si="4"/>
+        <v>7.1753169098304564E-2</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276" s="3">
         <v>44866</v>
       </c>
       <c r="B276" s="1">
         <v>4.218</v>
       </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C276">
+        <f t="shared" si="4"/>
+        <v>0.81261950286806417</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277" s="3">
         <v>44896</v>
       </c>
       <c r="B277" s="1">
         <v>4.2110000000000003</v>
       </c>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C277">
+        <f t="shared" si="4"/>
+        <v>-0.16595542911331609</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278" s="3">
         <v>44927</v>
       </c>
       <c r="B278" s="1">
         <v>4.2039999999999997</v>
       </c>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C278">
+        <f t="shared" si="4"/>
+        <v>-0.1662312989788782</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A279" s="3">
         <v>44958</v>
       </c>
       <c r="B279" s="1">
         <v>4.1630000000000003</v>
       </c>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C279">
+        <f t="shared" si="4"/>
+        <v>-0.97526165556611533</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A280" s="3">
         <v>44986</v>
       </c>
       <c r="B280" s="1">
         <v>4.0979999999999999</v>
       </c>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C280">
+        <f t="shared" si="4"/>
+        <v>-1.5613740091280419</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281" s="3">
         <v>45017</v>
       </c>
       <c r="B281" s="1">
         <v>4.0419999999999998</v>
+      </c>
+      <c r="C281">
+        <f t="shared" si="4"/>
+        <v>-1.366520253782334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>